<commit_message>
Created walkthrough for making new predictions
</commit_message>
<xml_diff>
--- a/Predictors/Han_et al.2012_AlbuminProteinBinding_Data.xlsx
+++ b/Predictors/Han_et al.2012_AlbuminProteinBinding_Data.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Lab\NCCT_ExpoCast\ExpoCast2019\TK_QSAR_PFAS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwambaug\git\CompTox-PFASHalfLife\Predictors\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E92D5749-805E-4A10-BFBB-943B43212EBB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD455423-FF4E-4766-9B30-90CC79321191}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CCAFB240-5043-45BE-AD97-7C27D3ADFD2C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{CCAFB240-5043-45BE-AD97-7C27D3ADFD2C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +23,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="34">
   <si>
     <t>Species</t>
   </si>
@@ -97,6 +102,42 @@
   </si>
   <si>
     <t>ChemicalAbbreviation</t>
+  </si>
+  <si>
+    <t>DTXSID</t>
+  </si>
+  <si>
+    <t>CASRN</t>
+  </si>
+  <si>
+    <t>DTXSID60873015</t>
+  </si>
+  <si>
+    <t>45187-15-3</t>
+  </si>
+  <si>
+    <t>DTXSID1037303</t>
+  </si>
+  <si>
+    <t>375-85-9</t>
+  </si>
+  <si>
+    <t>DTXSID8031865</t>
+  </si>
+  <si>
+    <t>335-67-1</t>
+  </si>
+  <si>
+    <t>DTXSID8031863</t>
+  </si>
+  <si>
+    <t>375-95-1</t>
+  </si>
+  <si>
+    <t>DTXSID3031860</t>
+  </si>
+  <si>
+    <t>335-76-2</t>
   </si>
 </sst>
 </file>
@@ -113,9 +154,8 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Lucida Console"/>
-      <family val="3"/>
+      <color indexed="12"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -141,9 +181,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -458,219 +496,287 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07CE2A76-BB84-4A3B-BF6B-0B885D0DC56D}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="28.42578125" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>21</v>
       </c>
       <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>14</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="1">
+      <c r="G2" s="1">
         <v>1100000</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
         <v>17</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="1">
+      <c r="G3" s="1">
         <v>9400</v>
       </c>
-      <c r="F3">
+      <c r="H3">
         <v>1.44</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="1">
+      <c r="G4" s="1">
         <v>44000</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
         <v>18</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" t="s">
         <v>10</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="1">
+      <c r="G5" s="1">
         <v>2800</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
         <v>18</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" t="s">
         <v>4</v>
       </c>
-      <c r="D6" t="s">
+      <c r="F6" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="1">
+      <c r="G6" s="1">
         <v>22000</v>
       </c>
-      <c r="F6">
+      <c r="H6">
         <v>1.9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
         <v>19</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" t="s">
         <v>9</v>
       </c>
-      <c r="D7" t="s">
+      <c r="F7" t="s">
         <v>5</v>
       </c>
-      <c r="E7">
+      <c r="G7">
         <f>AVERAGE(600000, 900)</f>
         <v>300450</v>
       </c>
-      <c r="F7" t="s">
+      <c r="H7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
         <v>19</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" t="s">
         <v>4</v>
       </c>
-      <c r="D8" t="s">
+      <c r="F8" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="1">
+      <c r="G8" s="1">
         <v>26000</v>
       </c>
-      <c r="F8">
+      <c r="H8">
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" t="s">
         <v>20</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" t="s">
         <v>9</v>
       </c>
-      <c r="D9" t="s">
+      <c r="F9" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="1">
+      <c r="G9" s="1">
         <v>690000</v>
       </c>
-      <c r="F9" t="s">
+      <c r="H9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" t="s">
         <v>20</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" t="s">
         <v>4</v>
       </c>
-      <c r="D10" t="s">
+      <c r="F10" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="1">
+      <c r="G10" s="1">
         <v>48000</v>
       </c>
-      <c r="F10" t="s">
+      <c r="H10" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{87429CFA-ABE3-4B73-98F2-5FBF9F68B953}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{8C2D54E7-1FB8-431E-94FC-700DA2AC1758}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{5AB16836-9478-4DDF-AF58-F4C18900451F}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{3FEFDD9B-3F3D-4712-8ACA-13C29DFD87F2}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{E5E03837-163B-4F60-A329-59FB27E0906D}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{13DC0510-E6FA-49B9-A0D1-AF3191F5C2FC}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{3889060E-86AF-4046-BAD1-08FCBD0848AE}"/>
+    <hyperlink ref="B9" r:id="rId8" xr:uid="{9F970A27-668D-4EAA-BD93-657BDD174A56}"/>
+    <hyperlink ref="B10" r:id="rId9" xr:uid="{6DFBF298-F6CC-4D07-93CC-C289E041AF15}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>